<commit_message>
vault backup: 2024-03-09 23:03:25
</commit_message>
<xml_diff>
--- a/cs-ai/工程心理学/测量作业.xlsx
+++ b/cs-ai/工程心理学/测量作业.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC5BDE4-5FFA-469B-AAD6-1707B4800BB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +19,97 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+  <si>
+    <t>测量时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测量地点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测量项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAeq,T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西1一楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西1二楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>西1四楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>余杭塘路</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LApeak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测量结果dB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仪器是否校准：是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>气象条件：晴，无风</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期：3月9日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测定人员：马琦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仪器型号：AWA5688</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测点序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -37,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -45,15 +129,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +470,304 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4">
+        <v>43.1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.64513888888888882</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44.8</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>70.7</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4">
+        <v>69.3</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>80.8</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.64513888888888882</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4">
+        <v>79.5</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4">
+        <v>82.4</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4">
+        <v>107.8</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4">
+        <v>93.4</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="7">
+        <v>90.5</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>